<commit_message>
remote download wait time, store selectors in variables
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
   <si>
     <t>Name</t>
   </si>
@@ -267,15 +267,6 @@
   </si>
   <si>
     <t>The name of the storage bucket</t>
-  </si>
-  <si>
-    <t>BuyWaysDepartmentApprovers_DownloadWaitTime</t>
-  </si>
-  <si>
-    <t>DownloadWaitTime</t>
-  </si>
-  <si>
-    <t>The amount of time (in minutes) to wait for the csv file to download</t>
   </si>
   <si>
     <t>BuyWaysDepartmentApprovers_BuyWaysLogoutURL</t>
@@ -2953,10 +2944,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3146,7 +3137,7 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B12" t="s">
         <v>84</v>
@@ -3155,7 +3146,7 @@
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -3172,20 +3163,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C14" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" t="s">
-        <v>91</v>
-      </c>
-    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -4169,7 +4147,6 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
extract business logic workflows, refactor buyways login arguments, condense email sending
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsardonini\Documents\UiPath\BuywaysDepartmentApprovers\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsardonini\Documents\UiPath\BuywaysDepartmentApproversReportGenerationAndUpload\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="2"/>
+    <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
   <si>
     <t>Name</t>
   </si>
@@ -212,9 +212,6 @@
     <t>The name of the asset in Orchestrator for logging into email</t>
   </si>
   <si>
-    <t>BuywaysDepartmentApproversEmailCredentials</t>
-  </si>
-  <si>
     <t>BuyWaysLoginCredentials</t>
   </si>
   <si>
@@ -294,6 +291,18 @@
   </si>
   <si>
     <t>SendSlackNotificationEmail</t>
+  </si>
+  <si>
+    <t>BuyWaysDepartmentApprovers_BuyWaysURL</t>
+  </si>
+  <si>
+    <t>The name of the asset in Orchestrator that holds the Buyways login URL</t>
+  </si>
+  <si>
+    <t>BuyWaysLoginURLAssetName</t>
+  </si>
+  <si>
+    <t>BuyWaysDepartmentApproversEmailCredentials</t>
   </si>
 </sst>
 </file>
@@ -1753,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1948,7 +1957,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
         <v>57</v>
@@ -1959,16 +1968,26 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" t="s">
         <v>63</v>
       </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" t="s">
-        <v>64</v>
-      </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2946,7 +2965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -3053,114 +3072,114 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>72</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" t="s">
         <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
change email to use send email library, remove unused email config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -197,21 +197,6 @@
     <t>The email to send notifications to</t>
   </si>
   <si>
-    <t>BuyWaysDepartmentApprovers_EmailCredentials</t>
-  </si>
-  <si>
-    <t>BuyWaysDepartmentApprovers_ExchangeServerURL</t>
-  </si>
-  <si>
-    <t>ExchangeServerURL</t>
-  </si>
-  <si>
-    <t>The URL for the exchange server</t>
-  </si>
-  <si>
-    <t>The name of the asset in Orchestrator for logging into email</t>
-  </si>
-  <si>
     <t>BuyWaysLoginCredentials</t>
   </si>
   <si>
@@ -300,9 +285,6 @@
   </si>
   <si>
     <t>BuyWaysLoginURLAssetName</t>
-  </si>
-  <si>
-    <t>BuyWaysDepartmentApproversEmailCredentials</t>
   </si>
 </sst>
 </file>
@@ -1760,10 +1742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z988"/>
+  <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1957,37 +1939,27 @@
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C21" t="s">
-        <v>90</v>
-      </c>
-    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2954,7 +2926,6 @@
     <row r="985" ht="14.25" customHeight="1"/>
     <row r="986" ht="14.25" customHeight="1"/>
     <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2963,10 +2934,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3058,44 +3029,44 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>45</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3103,85 +3074,72 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
         <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C9" t="s">
         <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>45</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
         <v>45</v>
       </c>
       <c r="D12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
-    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4165,7 +4123,6 @@
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>